<commit_message>
added sla column to harvest datashee
</commit_message>
<xml_diff>
--- a/Data/structural/harvest_datasheet.xlsx
+++ b/Data/structural/harvest_datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4de34fb287247afc/Desktop/Git/variability_ms_thesis/Data/structural/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="391" documentId="8_{6DFACC2F-227F-4DE8-8D90-CEBBC8BA0B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C3A6F67-0BF9-412D-8549-598B7F838E85}"/>
+  <xr:revisionPtr revIDLastSave="393" documentId="8_{6DFACC2F-227F-4DE8-8D90-CEBBC8BA0B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48018EFF-0499-4A1B-A1FF-CB14EB57EA75}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{83655F9C-250C-451D-A898-839DE6E3EBE4}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{83655F9C-250C-451D-A898-839DE6E3EBE4}"/>
   </bookViews>
   <sheets>
     <sheet name="harvest_day" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>plant_ID</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>combined_leaf_areas (cm^2)</t>
+  </si>
+  <si>
+    <t>SLA_focal</t>
   </si>
 </sst>
 </file>
@@ -666,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E122E7-7223-4CCF-A57A-9C3DAA94A927}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,9 +688,10 @@
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="20.54296875" customWidth="1"/>
     <col min="11" max="11" width="25.81640625" customWidth="1"/>
+    <col min="12" max="12" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,8 +725,11 @@
       <c r="K1" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -755,8 +762,11 @@
         <f>H2+I2+J2</f>
         <v>474.29999999999995</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>264.77095939999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -789,8 +799,11 @@
         <f t="shared" ref="K3:K61" si="1">H3+I3+J3</f>
         <v>422.98700000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3" s="5">
+        <v>277.8731343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -823,8 +836,11 @@
         <f t="shared" si="1"/>
         <v>487.40199999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>319.72162739999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -857,8 +873,11 @@
         <f t="shared" si="1"/>
         <v>511.04</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5" s="5">
+        <v>244.12356320000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -891,8 +910,11 @@
         <f t="shared" si="1"/>
         <v>526.21500000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>283.33035710000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -925,8 +947,11 @@
         <f t="shared" si="1"/>
         <v>883.07</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7" s="5">
+        <v>223.55501219999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -959,8 +984,11 @@
         <f t="shared" si="1"/>
         <v>601.529</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>241.34086099999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -993,8 +1021,11 @@
         <f t="shared" si="1"/>
         <v>530.02200000000005</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9" s="5">
+        <v>280.85088459999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1027,8 +1058,11 @@
         <f t="shared" si="1"/>
         <v>498.209</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>325.2873563</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1061,8 +1095,11 @@
         <f t="shared" si="1"/>
         <v>512.38099999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11" s="5">
+        <v>211.5696203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1095,8 +1132,11 @@
         <f t="shared" si="1"/>
         <v>605.70400000000006</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>275.36694319999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1129,8 +1169,11 @@
         <f t="shared" si="1"/>
         <v>621.71900000000005</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13" s="5">
+        <v>238.82316700000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1163,8 +1206,11 @@
         <f t="shared" si="1"/>
         <v>617.97500000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>262.5930851</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -1197,8 +1243,11 @@
         <f t="shared" si="1"/>
         <v>538.71500000000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15" s="5">
+        <v>284.12444440000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1231,8 +1280,11 @@
         <f t="shared" si="1"/>
         <v>388.98899999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L16">
+        <v>299.94928149999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
@@ -1265,8 +1317,11 @@
         <f t="shared" si="1"/>
         <v>333.45699999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17" s="5">
+        <v>341.27966980000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1299,8 +1354,11 @@
         <f t="shared" si="1"/>
         <v>397.512</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>285.00408160000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -1333,8 +1391,11 @@
         <f t="shared" si="1"/>
         <v>286.21999999999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L19" s="5">
+        <v>333.77483439999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1367,8 +1428,11 @@
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L20">
+        <v>347.36785329999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1401,8 +1465,11 @@
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21" s="5">
+        <v>333.44978170000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1435,8 +1502,11 @@
         <f t="shared" si="1"/>
         <v>936.89499999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L22">
+        <v>224.3722564</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -1469,8 +1539,11 @@
         <f t="shared" si="1"/>
         <v>650.67700000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L23" s="5">
+        <v>329.81160510000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1503,8 +1576,11 @@
         <f t="shared" si="1"/>
         <v>682.55100000000004</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L24">
+        <v>296.03155340000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
@@ -1537,8 +1613,11 @@
         <f t="shared" si="1"/>
         <v>936.08299999999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L25" s="5">
+        <v>215.73488370000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1571,8 +1650,11 @@
         <f t="shared" si="1"/>
         <v>1055.25</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L26">
+        <v>212.93056809999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
@@ -1605,8 +1687,11 @@
         <f t="shared" si="1"/>
         <v>811.70600000000002</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L27" s="5">
+        <v>238.4995112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1639,8 +1724,11 @@
         <f t="shared" si="1"/>
         <v>632.23099999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L28">
+        <v>326.88958009999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
@@ -1673,8 +1761,11 @@
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L29" s="5">
+        <v>290.70403279999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1707,8 +1798,11 @@
         <f t="shared" si="1"/>
         <v>420.714</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L30">
+        <v>362.70758119999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
@@ -1741,8 +1835,11 @@
         <f t="shared" si="1"/>
         <v>543.43299999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L31" s="5">
+        <v>277.15582449999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1775,8 +1872,11 @@
         <f t="shared" si="1"/>
         <v>688.24300000000005</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L32">
+        <v>226.25986080000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
@@ -1809,8 +1909,11 @@
         <f t="shared" si="1"/>
         <v>468.99900000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L33" s="5">
+        <v>268.96243290000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1843,8 +1946,11 @@
         <f t="shared" si="1"/>
         <v>338.56699999999995</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L34">
+        <v>353.21671529999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
@@ -1877,8 +1983,11 @@
         <f t="shared" si="1"/>
         <v>394.64300000000003</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L35" s="5">
+        <v>327.48695650000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1911,8 +2020,11 @@
         <f t="shared" si="1"/>
         <v>444.298</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L36">
+        <v>273.89583329999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
@@ -1945,8 +2057,11 @@
         <f t="shared" si="1"/>
         <v>512.02199999999993</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L37" s="5">
+        <v>269.50784590000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1979,8 +2094,11 @@
         <f t="shared" si="1"/>
         <v>626.226</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L38">
+        <v>195.1815642</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>38</v>
       </c>
@@ -2013,8 +2131,11 @@
         <f t="shared" si="1"/>
         <v>540.70399999999995</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L39" s="5">
+        <v>251.65618449999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2047,8 +2168,11 @@
         <f t="shared" si="1"/>
         <v>635.35299999999995</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L40">
+        <v>197.5708314</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
@@ -2081,8 +2205,11 @@
         <f t="shared" si="1"/>
         <v>469.43899999999996</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L41" s="5">
+        <v>335.85629920000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2115,8 +2242,11 @@
         <f t="shared" si="1"/>
         <v>451.03499999999997</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L42">
+        <v>302.34732819999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
@@ -2149,8 +2279,11 @@
         <f t="shared" si="1"/>
         <v>538.48</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L43" s="5">
+        <v>283.56313990000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2183,8 +2316,11 @@
         <f t="shared" si="1"/>
         <v>441.51199999999994</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L44">
+        <v>301.8604651</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>44</v>
       </c>
@@ -2217,8 +2353,11 @@
         <f t="shared" si="1"/>
         <v>388.68699999999995</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L45" s="5">
+        <v>327.28971960000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2251,8 +2390,11 @@
         <f t="shared" si="1"/>
         <v>505.654</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L46">
+        <v>271.60000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
@@ -2285,8 +2427,11 @@
         <f t="shared" si="1"/>
         <v>713</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L47" s="5">
+        <v>289.25642429999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2319,8 +2464,11 @@
         <f t="shared" si="1"/>
         <v>459.43799999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L48">
+        <v>288.23715920000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>48</v>
       </c>
@@ -2353,8 +2501,11 @@
         <f t="shared" si="1"/>
         <v>657.14499999999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L49" s="5">
+        <v>249.72274440000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2387,8 +2538,11 @@
         <f t="shared" si="1"/>
         <v>381.57599999999996</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L50">
+        <v>318.85462560000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>50</v>
       </c>
@@ -2421,8 +2575,11 @@
         <f t="shared" si="1"/>
         <v>478.03300000000002</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L51" s="5">
+        <v>268.05910540000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2455,8 +2612,11 @@
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L52">
+        <v>264.42801559999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>52</v>
       </c>
@@ -2489,8 +2649,11 @@
         <f t="shared" si="1"/>
         <v>667.47800000000007</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L53" s="5">
+        <v>239.8499674</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2523,8 +2686,11 @@
         <f t="shared" si="1"/>
         <v>523.99599999999998</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L54">
+        <v>250.7137491</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>54</v>
       </c>
@@ -2557,8 +2723,11 @@
         <f t="shared" si="1"/>
         <v>523.80399999999997</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L55" s="5">
+        <v>287.78741869999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2591,8 +2760,11 @@
         <f t="shared" si="1"/>
         <v>464.096</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L56">
+        <v>298.67562379999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>56</v>
       </c>
@@ -2625,8 +2797,11 @@
         <f t="shared" si="1"/>
         <v>582.81899999999996</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L57" s="5">
+        <v>223.5810056</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2659,8 +2834,11 @@
         <f t="shared" si="1"/>
         <v>578.28899999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L58">
+        <v>256.61100800000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>58</v>
       </c>
@@ -2693,8 +2871,11 @@
         <f t="shared" si="1"/>
         <v>440.17500000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L59" s="5">
+        <v>224.21785940000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2727,8 +2908,11 @@
         <f t="shared" si="1"/>
         <v>586.43100000000004</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L60">
+        <v>269.3090909</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>60</v>
       </c>
@@ -2760,6 +2944,9 @@
       <c r="K61" s="5">
         <f t="shared" si="1"/>
         <v>458.54500000000002</v>
+      </c>
+      <c r="L61" s="5">
+        <v>266.81818179999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>